<commit_message>
compute distance travelled per individual
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanneeverling/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\sanne-thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3B6788CC-A622-6F44-A9D1-B5D195D0DA6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F194B13-74C4-4926-BFBF-0D1D37DCB00D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="960" windowWidth="25040" windowHeight="14500" xr2:uid="{250E1811-A185-AF47-A5FD-F1914561EB1A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{250E1811-A185-AF47-A5FD-F1914561EB1A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,6 +26,7 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -519,9 +520,9 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>42</v>
       </c>
@@ -598,7 +599,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -660,7 +661,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -722,7 +723,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -784,7 +785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -846,7 +847,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>

</xml_diff>